<commit_message>
added title screen to game to reuse as pause menu buttons dont work
</commit_message>
<xml_diff>
--- a/Project Documents/HELLSCENT 2023 WORK BREAKDOWN STRUCTURE.xlsx
+++ b/Project Documents/HELLSCENT 2023 WORK BREAKDOWN STRUCTURE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s-knotwella\TopDown\Project Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s-wongg\TopDown\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921EDC47-0AF7-4342-914E-DB304CE78EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5ACF22D-C7CC-41DC-B08A-5A267C4CE435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{262C9EA2-0170-48E3-BC48-848692BFFBE2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="158">
   <si>
     <t>Owner</t>
   </si>
@@ -491,6 +491,45 @@
   </si>
   <si>
     <t>Made button in options menu for attack keybinds. Wrote script to show custom keybinds on button and store in PlayerPrefs as a string. Saves keybinds even after closing game. </t>
+  </si>
+  <si>
+    <t>Custom pick up item and swap item button </t>
+  </si>
+  <si>
+    <t>Created buttons for pick up item and swap item on options menu. Added to script but doesn’t save keybinds separately. </t>
+  </si>
+  <si>
+    <t>Saving multiple keybinds in Playerprefs </t>
+  </si>
+  <si>
+    <t>Edited Script to have separate strings in Playerprefs for each of the three keybinds.  </t>
+  </si>
+  <si>
+    <t>Player controls using custom keybinds </t>
+  </si>
+  <si>
+    <t>Implemented custom keybinds into playercontroller script. Doesn’t work because it doesn’t recognize string names of keybinds stored in Playerprefs. </t>
+  </si>
+  <si>
+    <t>Saving keybinds as ints </t>
+  </si>
+  <si>
+    <t>Saved keybinds as ints in Playerprefs because formatting doesn’t get messed up and Input.GetKeyDown can recognize ints as input. Now displays ints instead of names of keys in options menu. </t>
+  </si>
+  <si>
+    <t>Separating player keybind with displayed keybind in options menu </t>
+  </si>
+  <si>
+    <t>Created separate values for the int format of keybind and string format of keybind. Uses the int in playercontroller and displays string in options menu. </t>
+  </si>
+  <si>
+    <t>Pause game</t>
+  </si>
+  <si>
+    <t>Gameplay &amp; Player controls</t>
+  </si>
+  <si>
+    <t>User can press escape to pause the game(anything that uses time). Doesn’t stop update() from running</t>
   </si>
 </sst>
 </file>
@@ -806,7 +845,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -871,6 +910,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -898,41 +979,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,11 +1299,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E01AB7-C3E4-4259-857A-9FD7B615EF5F}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39:F40"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1680,218 +1731,218 @@
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="41" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="22"/>
+      <c r="H19" s="36"/>
     </row>
     <row r="20" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
       <c r="G20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="37"/>
     </row>
     <row r="21" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="27" t="s">
+      <c r="C21" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="41" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="36"/>
     </row>
     <row r="22" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
       <c r="G22" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="30"/>
+      <c r="H22" s="44"/>
     </row>
     <row r="23" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="30"/>
+      <c r="H23" s="44"/>
     </row>
     <row r="24" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="30"/>
+      <c r="H24" s="44"/>
     </row>
     <row r="25" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="23"/>
+      <c r="H25" s="37"/>
     </row>
     <row r="26" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="27" t="s">
+      <c r="C26" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="27" t="s">
+      <c r="F26" s="41" t="s">
         <v>52</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="22"/>
+      <c r="H26" s="36"/>
     </row>
     <row r="27" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
       <c r="G27" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="23"/>
+      <c r="H27" s="37"/>
     </row>
     <row r="28" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="41" t="s">
         <v>57</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="36"/>
     </row>
     <row r="29" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
       <c r="G29" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H29" s="23"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="27" t="s">
+      <c r="C30" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="41" t="s">
         <v>60</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="22"/>
+      <c r="H30" s="36"/>
     </row>
     <row r="31" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
       <c r="F31" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="29"/>
-      <c r="H31" s="23"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="37"/>
     </row>
     <row r="32" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
@@ -1918,38 +1969,38 @@
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="27" t="s">
+      <c r="C33" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="27" t="s">
+      <c r="F33" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="27" t="s">
+      <c r="G33" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H33" s="22"/>
+      <c r="H33" s="36"/>
     </row>
     <row r="34" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="23"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="37"/>
     </row>
     <row r="35" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
@@ -2000,72 +2051,72 @@
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="27" t="s">
+      <c r="C37" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="41" t="s">
         <v>76</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="H37" s="22"/>
+      <c r="H37" s="36"/>
     </row>
     <row r="38" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
       <c r="G38" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H38" s="23"/>
+      <c r="H38" s="37"/>
     </row>
     <row r="39" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="27" t="s">
+      <c r="C39" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="27" t="s">
+      <c r="F39" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="G39" s="27"/>
-      <c r="H39" s="22"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="36"/>
     </row>
     <row r="40" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="23"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="37"/>
     </row>
     <row r="41" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -2341,94 +2392,94 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="35" t="s">
+      <c r="C53" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="F53" s="35" t="s">
+      <c r="F53" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="G53" s="36" t="s">
+      <c r="G53" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="32" t="s">
+      <c r="B54" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="31" t="s">
+      <c r="C54" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="F54" s="31" t="s">
+      <c r="F54" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="G54" s="38" t="s">
+      <c r="G54" s="29" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="37" t="s">
+      <c r="A55" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="32" t="s">
+      <c r="B55" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="31" t="s">
+      <c r="C55" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="F55" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="G55" s="38" t="s">
+      <c r="G55" s="29" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="31" t="s">
+      <c r="C56" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F56" s="31" t="s">
+      <c r="F56" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="G56" s="38" t="s">
+      <c r="G56" s="29" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2436,19 +2487,19 @@
       <c r="A57" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B57" s="32" t="s">
+      <c r="B57" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="32" t="s">
+      <c r="C57" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F57" s="32" t="s">
+      <c r="F57" s="23" t="s">
         <v>129</v>
       </c>
       <c r="G57" s="7" t="s">
@@ -2459,19 +2510,19 @@
       <c r="A58" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="32" t="s">
+      <c r="C58" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F58" s="32" t="s">
+      <c r="F58" s="23" t="s">
         <v>131</v>
       </c>
       <c r="G58" s="7" t="s">
@@ -2482,19 +2533,19 @@
       <c r="A59" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="32" t="s">
+      <c r="B59" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="32" t="s">
+      <c r="C59" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F59" s="32" t="s">
+      <c r="F59" s="23" t="s">
         <v>133</v>
       </c>
       <c r="G59" s="7" t="s">
@@ -2502,25 +2553,25 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="32" t="s">
+      <c r="B60" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="31" t="s">
+      <c r="C60" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F60" s="31" t="s">
+      <c r="F60" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="G60" s="38" t="s">
+      <c r="G60" s="29" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2528,19 +2579,19 @@
       <c r="A61" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="32" t="s">
+      <c r="B61" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="32" t="s">
+      <c r="C61" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="32" t="s">
+      <c r="F61" s="23" t="s">
         <v>137</v>
       </c>
       <c r="G61" s="7" t="s">
@@ -2551,46 +2602,184 @@
       <c r="A62" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B62" s="32" t="s">
+      <c r="B62" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C62" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="32" t="s">
+      <c r="C62" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E62" s="32" t="s">
+      <c r="E62" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F62" s="32" t="s">
+      <c r="F62" s="23" t="s">
         <v>140</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="39" t="s">
+    <row r="63" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B63" s="40" t="s">
+      <c r="B63" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="41" t="s">
+      <c r="C63" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="F63" s="41" t="s">
+      <c r="F63" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="G63" s="42" t="s">
+      <c r="G63" s="33" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" s="23">
+        <v>3</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" s="23">
+        <v>3</v>
+      </c>
+      <c r="C66" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="F66" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="G66" s="35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="25">
+        <v>2</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F67" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="F68" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="G68" s="35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="10">
+        <v>1</v>
+      </c>
+      <c r="C69" s="19">
+        <v>1</v>
+      </c>
+      <c r="D69" s="10">
+        <v>0</v>
+      </c>
+      <c r="E69" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="G69" s="21" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Game Design Document
</commit_message>
<xml_diff>
--- a/Project Documents/HELLSCENT 2023 WORK BREAKDOWN STRUCTURE.xlsx
+++ b/Project Documents/HELLSCENT 2023 WORK BREAKDOWN STRUCTURE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s-knotwella\TopDown\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921EDC47-0AF7-4342-914E-DB304CE78EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFD65F3-3CD1-4685-8E4B-EF7FA9A0F97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{262C9EA2-0170-48E3-BC48-848692BFFBE2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="147">
   <si>
     <t>Owner</t>
   </si>
@@ -491,6 +491,12 @@
   </si>
   <si>
     <t>Made button in options menu for attack keybinds. Wrote script to show custom keybinds on button and store in PlayerPrefs as a string. Saves keybinds even after closing game. </t>
+  </si>
+  <si>
+    <t>Game Manager</t>
+  </si>
+  <si>
+    <t>Portal to Next Level</t>
   </si>
 </sst>
 </file>
@@ -806,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -871,6 +877,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -880,59 +922,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,11 +1257,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E01AB7-C3E4-4259-857A-9FD7B615EF5F}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39:F40"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1680,218 +1689,218 @@
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="38" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="22"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
       <c r="G20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="27" t="s">
+      <c r="C21" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="38" t="s">
         <v>45</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
       <c r="G22" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="30"/>
+      <c r="H22" s="42"/>
     </row>
     <row r="23" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="30"/>
+      <c r="H23" s="42"/>
     </row>
     <row r="24" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
       <c r="G24" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="30"/>
+      <c r="H24" s="42"/>
     </row>
     <row r="25" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="23"/>
+      <c r="H25" s="35"/>
     </row>
     <row r="26" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="27" t="s">
+      <c r="C26" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="27" t="s">
+      <c r="F26" s="38" t="s">
         <v>52</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="22"/>
+      <c r="H26" s="34"/>
     </row>
     <row r="27" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="23"/>
+      <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="38" t="s">
         <v>57</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H29" s="23"/>
+      <c r="H29" s="35"/>
     </row>
     <row r="30" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="27" t="s">
+      <c r="C30" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="38" t="s">
         <v>60</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="22"/>
+      <c r="H30" s="34"/>
     </row>
     <row r="31" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
       <c r="F31" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="29"/>
-      <c r="H31" s="23"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="35"/>
     </row>
     <row r="32" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
@@ -1918,38 +1927,38 @@
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="27" t="s">
+      <c r="C33" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="27" t="s">
+      <c r="F33" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="27" t="s">
+      <c r="G33" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="H33" s="22"/>
+      <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="23"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="35"/>
     </row>
     <row r="35" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
@@ -2000,72 +2009,72 @@
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="27" t="s">
+      <c r="C37" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="38" t="s">
         <v>76</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="H37" s="22"/>
+      <c r="H37" s="34"/>
     </row>
     <row r="38" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
       <c r="G38" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H38" s="23"/>
+      <c r="H38" s="35"/>
     </row>
     <row r="39" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="27" t="s">
+      <c r="C39" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="27" t="s">
+      <c r="F39" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="G39" s="27"/>
-      <c r="H39" s="22"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="34"/>
     </row>
     <row r="40" spans="1:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="23"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="35"/>
     </row>
     <row r="41" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -2341,94 +2350,94 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="35" t="s">
+      <c r="C53" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="F53" s="35" t="s">
+      <c r="F53" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="G53" s="36" t="s">
+      <c r="G53" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="32" t="s">
+      <c r="B54" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="31" t="s">
+      <c r="C54" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="F54" s="31" t="s">
+      <c r="F54" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="G54" s="38" t="s">
+      <c r="G54" s="29" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="37" t="s">
+      <c r="A55" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="32" t="s">
+      <c r="B55" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="31" t="s">
+      <c r="C55" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="F55" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="G55" s="38" t="s">
+      <c r="G55" s="29" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="31" t="s">
+      <c r="C56" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F56" s="31" t="s">
+      <c r="F56" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="G56" s="38" t="s">
+      <c r="G56" s="29" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2436,19 +2445,19 @@
       <c r="A57" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B57" s="32" t="s">
+      <c r="B57" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="32" t="s">
+      <c r="C57" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F57" s="32" t="s">
+      <c r="F57" s="23" t="s">
         <v>129</v>
       </c>
       <c r="G57" s="7" t="s">
@@ -2459,19 +2468,19 @@
       <c r="A58" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="32" t="s">
+      <c r="C58" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F58" s="32" t="s">
+      <c r="F58" s="23" t="s">
         <v>131</v>
       </c>
       <c r="G58" s="7" t="s">
@@ -2482,19 +2491,19 @@
       <c r="A59" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="32" t="s">
+      <c r="B59" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="32" t="s">
+      <c r="C59" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F59" s="32" t="s">
+      <c r="F59" s="23" t="s">
         <v>133</v>
       </c>
       <c r="G59" s="7" t="s">
@@ -2502,25 +2511,25 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="32" t="s">
+      <c r="B60" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="31" t="s">
+      <c r="C60" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F60" s="31" t="s">
+      <c r="F60" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="G60" s="38" t="s">
+      <c r="G60" s="29" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2528,19 +2537,19 @@
       <c r="A61" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="32" t="s">
+      <c r="B61" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="32" t="s">
+      <c r="C61" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="32" t="s">
+      <c r="F61" s="23" t="s">
         <v>137</v>
       </c>
       <c r="G61" s="7" t="s">
@@ -2551,19 +2560,19 @@
       <c r="A62" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B62" s="32" t="s">
+      <c r="B62" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C62" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="32" t="s">
+      <c r="C62" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E62" s="32" t="s">
+      <c r="E62" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F62" s="32" t="s">
+      <c r="F62" s="23" t="s">
         <v>140</v>
       </c>
       <c r="G62" s="7" t="s">
@@ -2571,30 +2580,90 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B63" s="40" t="s">
+      <c r="B63" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D63" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="41" t="s">
+      <c r="C63" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="F63" s="41" t="s">
+      <c r="F63" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="G63" s="42" t="s">
+      <c r="G63" s="33" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" s="10">
+        <v>3</v>
+      </c>
+      <c r="C64" s="19">
+        <v>1</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="E21:E25"/>
+    <mergeCell ref="F21:F25"/>
+    <mergeCell ref="H21:H25"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="G30:G31"/>
     <mergeCell ref="H37:H38"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
@@ -2610,49 +2679,6 @@
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="E37:E38"/>
     <mergeCell ref="F37:F38"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="E21:E25"/>
-    <mergeCell ref="F21:F25"/>
-    <mergeCell ref="H21:H25"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>